<commit_message>
Short update to files
Converted .xlsm to .csv. Added notes.
</commit_message>
<xml_diff>
--- a/PackageRenamer/PackageRenamer_BugDatabase.xlsx
+++ b/PackageRenamer/PackageRenamer_BugDatabase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Steps to Reproduce</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Fixed Status</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -94,13 +97,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,141 +418,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3B06ED-3974-4B14-8C63-F7D7ACBDDEBC}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>